<commit_message>
updated chart of account(add,edit and import) + partial update in journal entry
</commit_message>
<xml_diff>
--- a/public/extra/edit_excel/coa.xlsx
+++ b/public/extra/edit_excel/coa.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Account Code</t>
   </si>
   <si>
-    <t>Account Type</t>
-  </si>
-  <si>
     <t>Account Description</t>
   </si>
   <si>
@@ -34,17 +31,17 @@
     <t>Account Classification</t>
   </si>
   <si>
-    <t>Sub Account</t>
-  </si>
-  <si>
-    <t>Beginning Balance</t>
+    <t>Line Item</t>
+  </si>
+  <si>
+    <t>Cost Center Code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,20 +50,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,20 +73,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A2" sqref="A2:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,88 +407,29 @@
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
+      <c r="H1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>